<commit_message>
Update N2200_database - column title changing.xlsx
</commit_message>
<xml_diff>
--- a/db_feed/N2200/N2200_database - column title changing.xlsx
+++ b/db_feed/N2200/N2200_database - column title changing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myeongyeon Lee\Documents\GitHub\ofet-db\db_feed\N2200\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EFF035-612D-4FF8-8F7F-BFEDFC840DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79402E0B-FFC3-41AB-AB40-063AE7B061D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11445" yWindow="900" windowWidth="21600" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N2200_database - column title c" sheetId="1" r:id="rId1"/>
@@ -1526,7 +1526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BK28" sqref="BK28:BN29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3481,10 +3483,18 @@
       </c>
       <c r="BI15" s="1"/>
       <c r="BJ15" s="1"/>
-      <c r="BK15" s="1"/>
-      <c r="BL15" s="1"/>
-      <c r="BM15" s="1"/>
-      <c r="BN15" s="1"/>
+      <c r="BK15" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="BL15" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="BM15" s="1">
+        <v>208</v>
+      </c>
+      <c r="BN15" s="1">
+        <v>15.5</v>
+      </c>
       <c r="BO15" s="1"/>
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
@@ -3599,10 +3609,18 @@
       </c>
       <c r="BI16" s="1"/>
       <c r="BJ16" s="1"/>
-      <c r="BK16" s="1"/>
-      <c r="BL16" s="1"/>
-      <c r="BM16" s="1"/>
-      <c r="BN16" s="1"/>
+      <c r="BK16" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="BL16" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="BM16" s="1">
+        <v>208</v>
+      </c>
+      <c r="BN16" s="1">
+        <v>15.5</v>
+      </c>
       <c r="BO16" s="1"/>
       <c r="BP16" s="1"/>
       <c r="BQ16" s="1"/>
@@ -3717,10 +3735,18 @@
       </c>
       <c r="BI17" s="1"/>
       <c r="BJ17" s="1"/>
-      <c r="BK17" s="1"/>
-      <c r="BL17" s="1"/>
-      <c r="BM17" s="1"/>
-      <c r="BN17" s="1"/>
+      <c r="BK17" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="BL17" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="BM17" s="1">
+        <v>208</v>
+      </c>
+      <c r="BN17" s="1">
+        <v>15.5</v>
+      </c>
       <c r="BO17" s="1"/>
       <c r="BP17" s="1"/>
       <c r="BQ17" s="1"/>
@@ -3835,10 +3861,18 @@
       </c>
       <c r="BI18" s="1"/>
       <c r="BJ18" s="1"/>
-      <c r="BK18" s="1"/>
-      <c r="BL18" s="1"/>
-      <c r="BM18" s="1"/>
-      <c r="BN18" s="1"/>
+      <c r="BK18" s="1">
+        <v>24.6</v>
+      </c>
+      <c r="BL18" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM18" s="1">
+        <v>258</v>
+      </c>
+      <c r="BN18" s="1">
+        <v>20.399999999999999</v>
+      </c>
       <c r="BO18" s="1"/>
       <c r="BP18" s="1"/>
       <c r="BQ18" s="1"/>
@@ -3951,10 +3985,18 @@
       </c>
       <c r="BI19" s="1"/>
       <c r="BJ19" s="1"/>
-      <c r="BK19" s="1"/>
-      <c r="BL19" s="1"/>
-      <c r="BM19" s="1"/>
-      <c r="BN19" s="1"/>
+      <c r="BK19" s="1">
+        <v>24.6</v>
+      </c>
+      <c r="BL19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>258</v>
+      </c>
+      <c r="BN19" s="1">
+        <v>20.399999999999999</v>
+      </c>
       <c r="BO19" s="1"/>
       <c r="BP19" s="1"/>
       <c r="BQ19" s="1"/>
@@ -4067,10 +4109,18 @@
       </c>
       <c r="BI20" s="1"/>
       <c r="BJ20" s="1"/>
-      <c r="BK20" s="1"/>
-      <c r="BL20" s="1"/>
-      <c r="BM20" s="1"/>
-      <c r="BN20" s="1"/>
+      <c r="BK20" s="1">
+        <v>24.6</v>
+      </c>
+      <c r="BL20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>258</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>20.399999999999999</v>
+      </c>
       <c r="BO20" s="1"/>
       <c r="BP20" s="1"/>
       <c r="BQ20" s="1"/>
@@ -4183,10 +4233,18 @@
       </c>
       <c r="BI21" s="1"/>
       <c r="BJ21" s="1"/>
-      <c r="BK21" s="1"/>
-      <c r="BL21" s="1"/>
-      <c r="BM21" s="1"/>
-      <c r="BN21" s="1"/>
+      <c r="BK21" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="BL21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM21" s="1">
+        <v>243</v>
+      </c>
+      <c r="BN21" s="1">
+        <v>18.7</v>
+      </c>
       <c r="BO21" s="1"/>
       <c r="BP21" s="1"/>
       <c r="BQ21" s="1"/>
@@ -4299,10 +4357,18 @@
       </c>
       <c r="BI22" s="1"/>
       <c r="BJ22" s="1"/>
-      <c r="BK22" s="1"/>
-      <c r="BL22" s="1"/>
-      <c r="BM22" s="1"/>
-      <c r="BN22" s="1"/>
+      <c r="BK22" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="BL22" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM22" s="1">
+        <v>243</v>
+      </c>
+      <c r="BN22" s="1">
+        <v>18.7</v>
+      </c>
       <c r="BO22" s="1"/>
       <c r="BP22" s="1"/>
       <c r="BQ22" s="1"/>
@@ -4415,10 +4481,18 @@
       </c>
       <c r="BI23" s="1"/>
       <c r="BJ23" s="1"/>
-      <c r="BK23" s="1"/>
-      <c r="BL23" s="1"/>
-      <c r="BM23" s="1"/>
-      <c r="BN23" s="1"/>
+      <c r="BK23" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="BL23" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM23" s="1">
+        <v>243</v>
+      </c>
+      <c r="BN23" s="1">
+        <v>18.7</v>
+      </c>
       <c r="BO23" s="1"/>
       <c r="BP23" s="1"/>
       <c r="BQ23" s="1"/>
@@ -4531,10 +4605,18 @@
       </c>
       <c r="BI24" s="1"/>
       <c r="BJ24" s="1"/>
-      <c r="BK24" s="1"/>
-      <c r="BL24" s="1"/>
-      <c r="BM24" s="1"/>
-      <c r="BN24" s="1"/>
+      <c r="BK24" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL24" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM24" s="1">
+        <v>218</v>
+      </c>
+      <c r="BN24" s="1">
+        <v>20</v>
+      </c>
       <c r="BO24" s="1"/>
       <c r="BP24" s="1"/>
       <c r="BQ24" s="1"/>
@@ -4647,10 +4729,18 @@
       </c>
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
-      <c r="BL25" s="1"/>
-      <c r="BM25" s="1"/>
-      <c r="BN25" s="1"/>
+      <c r="BK25" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL25" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM25" s="1">
+        <v>218</v>
+      </c>
+      <c r="BN25" s="1">
+        <v>20</v>
+      </c>
       <c r="BO25" s="1"/>
       <c r="BP25" s="1"/>
       <c r="BQ25" s="1"/>
@@ -4763,10 +4853,18 @@
       </c>
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1"/>
-      <c r="BK26" s="1"/>
-      <c r="BL26" s="1"/>
-      <c r="BM26" s="1"/>
-      <c r="BN26" s="1"/>
+      <c r="BK26" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL26" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM26" s="1">
+        <v>218</v>
+      </c>
+      <c r="BN26" s="1">
+        <v>20</v>
+      </c>
       <c r="BO26" s="1"/>
       <c r="BP26" s="1"/>
       <c r="BQ26" s="1"/>
@@ -4879,10 +4977,18 @@
       </c>
       <c r="BI27" s="1"/>
       <c r="BJ27" s="1"/>
-      <c r="BK27" s="1"/>
-      <c r="BL27" s="1"/>
-      <c r="BM27" s="1"/>
-      <c r="BN27" s="1"/>
+      <c r="BK27" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL27" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM27" s="1">
+        <v>214</v>
+      </c>
+      <c r="BN27" s="1">
+        <v>18.100000000000001</v>
+      </c>
       <c r="BO27" s="1"/>
       <c r="BP27" s="1"/>
       <c r="BQ27" s="1"/>
@@ -4995,10 +5101,18 @@
       </c>
       <c r="BI28" s="1"/>
       <c r="BJ28" s="1"/>
-      <c r="BK28" s="1"/>
-      <c r="BL28" s="1"/>
-      <c r="BM28" s="1"/>
-      <c r="BN28" s="1"/>
+      <c r="BK28" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL28" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM28" s="1">
+        <v>214</v>
+      </c>
+      <c r="BN28" s="1">
+        <v>18.100000000000001</v>
+      </c>
       <c r="BO28" s="1"/>
       <c r="BP28" s="1"/>
       <c r="BQ28" s="1"/>
@@ -5111,10 +5225,18 @@
       </c>
       <c r="BI29" s="1"/>
       <c r="BJ29" s="1"/>
-      <c r="BK29" s="1"/>
-      <c r="BL29" s="1"/>
-      <c r="BM29" s="1"/>
-      <c r="BN29" s="1"/>
+      <c r="BK29" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BL29" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM29" s="1">
+        <v>214</v>
+      </c>
+      <c r="BN29" s="1">
+        <v>18.100000000000001</v>
+      </c>
       <c r="BO29" s="1"/>
       <c r="BP29" s="1"/>
       <c r="BQ29" s="1"/>

</xml_diff>